<commit_message>
homepage and calendar ui modified
</commit_message>
<xml_diff>
--- a/website/static/excel/Matches.xlsx
+++ b/website/static/excel/Matches.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>home_team</t>
   </si>
@@ -25,6 +25,9 @@
     <t>League_name</t>
   </si>
   <si>
+    <t>venue_name</t>
+  </si>
+  <si>
     <t>MALTEPESPOR</t>
   </si>
   <si>
@@ -34,7 +37,7 @@
     <t>1.GRUP</t>
   </si>
   <si>
-    <t/>
+    <t>-</t>
   </si>
   <si>
     <t>BEYKOZ ISHAKLI SPOR FAALIYETLERI</t>
@@ -211,7 +214,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -392,9 +395,6 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -426,6 +426,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -739,14 +742,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="18" width="38.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="45.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="18" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="38.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="45.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="15.290714285714287" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="18" width="35.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,331 +759,379 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+      <c r="C9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+        <v>31</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+        <v>33</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+        <v>35</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+        <v>37</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+        <v>39</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+        <v>41</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+        <v>43</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="C18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimization page wip and task 1111 and task 2222 done
</commit_message>
<xml_diff>
--- a/website/static/excel/Matches.xlsx
+++ b/website/static/excel/Matches.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+  <si>
+    <t>date</t>
+  </si>
   <si>
     <t>home_team</t>
   </si>
@@ -204,7 +207,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +218,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -286,6 +295,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -367,19 +383,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,44 +401,50 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -736,24 +754,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="38.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="17" width="45.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="18" width="35.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="19" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="38.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="45.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="20" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="21" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="21" width="35.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -762,377 +781,452 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5">
+        <v>45265</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>16</v>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5">
+        <v>45267</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>19</v>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>22</v>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="5">
+        <v>45267</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>25</v>
+      <c r="E9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>29</v>
       </c>
+      <c r="E10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="13"/>
+      <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="13"/>
+      <c r="C12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="13"/>
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="5">
+        <v>45266</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="13"/>
+      <c r="C14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="13"/>
+      <c r="C15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="13"/>
+      <c r="C16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="13"/>
+      <c r="C17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="15"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="D18" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5">
+        <v>45264</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="5">
+        <v>45270</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3"/>
+      <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="5">
+        <v>45265</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="3"/>
+      <c r="C21" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="5">
+        <v>45269</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="3"/>
+      <c r="C22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="5">
+        <v>45265</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="3"/>
+      <c r="C23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="A24" s="5">
+        <v>45269</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="3"/>
+      <c r="C24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
-      <c r="A25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="4" t="s">
+      <c r="A25" s="5">
+        <v>45265</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="3"/>
+      <c r="C25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>